<commit_message>
Start experiments report template
</commit_message>
<xml_diff>
--- a/experiments/results.xlsx
+++ b/experiments/results.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tridinc/Projects/genex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tridinc/Projects/genex/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset info" sheetId="1" r:id="rId1"/>
+    <sheet name="ItalyPowerDemand" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>Name</t>
   </si>
@@ -96,13 +97,100 @@
   </si>
   <si>
     <t>Download datasets</t>
+  </si>
+  <si>
+    <t>Sequence</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>k = 2</t>
+  </si>
+  <si>
+    <t>1 [4, 14]</t>
+  </si>
+  <si>
+    <t>17 [5, 10]</t>
+  </si>
+  <si>
+    <t>28 [11, 14]</t>
+  </si>
+  <si>
+    <t>60 [16, 18]</t>
+  </si>
+  <si>
+    <t>50 [2, 20]</t>
+  </si>
+  <si>
+    <t>76 [10, 24]</t>
+  </si>
+  <si>
+    <t>69 [0, 8]</t>
+  </si>
+  <si>
+    <t>55 [1, 13]</t>
+  </si>
+  <si>
+    <t>98 [16, 18]</t>
+  </si>
+  <si>
+    <t>83 [19, 22]</t>
+  </si>
+  <si>
+    <t>60 [22, 24]</t>
+  </si>
+  <si>
+    <t>66 [22, 24]</t>
+  </si>
+  <si>
+    <t>62 [9, 22]</t>
+  </si>
+  <si>
+    <t>25 [2, 24]</t>
+  </si>
+  <si>
+    <t>61 [12, 18]</t>
+  </si>
+  <si>
+    <t>72 [3, 13]</t>
+  </si>
+  <si>
+    <t>98 [17, 23]</t>
+  </si>
+  <si>
+    <t>92 [12, 14]</t>
+  </si>
+  <si>
+    <t>42 [8, 19]</t>
+  </si>
+  <si>
+    <t>79 [10, 21]</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>kSim</t>
+  </si>
+  <si>
+    <t>kSimRaw</t>
+  </si>
+  <si>
+    <t>Metrics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -126,6 +214,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -144,18 +255,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -434,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -691,4 +818,244 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="135" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="4">
+        <v>109</v>
+      </c>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>